<commit_message>
add initial version for dm-lookup widget
</commit_message>
<xml_diff>
--- a/wdc_libs/wdc-xlsx-converter/dataset-example.xlsx
+++ b/wdc_libs/wdc-xlsx-converter/dataset-example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="15120" windowHeight="7830" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="15120" windowHeight="7830" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="5" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4548" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4550" uniqueCount="552">
   <si>
     <t>Country Name</t>
   </si>
@@ -1674,6 +1674,9 @@
   </si>
   <si>
     <t>value.ua</t>
+  </si>
+  <si>
+    <t>https://www.whitehouse.gov/sites/default/files/immigration/icon_gdp_1.png</t>
   </si>
 </sst>
 </file>
@@ -2313,8 +2316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2322,7 +2325,7 @@
     <col min="1" max="1" width="30.42578125" style="5" customWidth="1"/>
     <col min="2" max="2" width="10.140625" style="5" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="5" customWidth="1"/>
     <col min="5" max="5" width="36.42578125" style="5" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" style="5" customWidth="1"/>
     <col min="7" max="16384" width="26.28515625" style="5"/>
@@ -2388,6 +2391,12 @@
       </c>
       <c r="C4" s="5" t="s">
         <v>531</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>525</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2437,8 +2446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
implements dictionary controller, add $lookup service
</commit_message>
<xml_diff>
--- a/wdc_libs/wdc-xlsx-converter/dataset-example.xlsx
+++ b/wdc_libs/wdc-xlsx-converter/dataset-example.xlsx
@@ -1655,9 +1655,6 @@
     <t>Світові індикатори розвитку</t>
   </si>
   <si>
-    <t>value.type</t>
-  </si>
-  <si>
     <t>value.label</t>
   </si>
   <si>
@@ -1677,6 +1674,9 @@
   </si>
   <si>
     <t>https://www.whitehouse.gov/sites/default/files/immigration/icon_gdp_1.png</t>
+  </si>
+  <si>
+    <t>type</t>
   </si>
 </sst>
 </file>
@@ -2317,7 +2317,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2331,24 +2331,24 @@
     <col min="7" max="16384" width="26.28515625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>551</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>544</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>545</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>546</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>547</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -2396,7 +2396,7 @@
         <v>525</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2461,10 +2461,10 @@
         <v>11</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>548</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>549</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="90" x14ac:dyDescent="0.25">

</xml_diff>